<commit_message>
Commit : 07/08/2018 Ajout :  Sprites Personnage lambda (80%) Image Map Sprite Interface Retouche interface Mémoire mis à jours (95%) Mémoire Anglais (format français) All sprite (.clip)
</commit_message>
<xml_diff>
--- a/DeathP_Doc/DonnéeInit.xlsx
+++ b/DeathP_Doc/DonnéeInit.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\DeathProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hihana\Desktop\DeathP_Git\DeathP_Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FDC446-5C92-4DCC-8C94-8CC616E0920D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16950" windowHeight="4590" xr2:uid="{9148EF4E-58C3-4C9E-A3A6-0771827E2A08}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22812" windowHeight="9182" xr2:uid="{9148EF4E-58C3-4C9E-A3A6-0771827E2A08}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2053,121 +2054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2201,6 +2088,24 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2213,16 +2118,112 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2543,24 +2544,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1DF257-2AA7-436E-BF39-4AB854BECBEB}">
   <dimension ref="A1:U101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="19"/>
-    <col min="10" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:21" ht="15.7" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2592,7 +2597,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
@@ -2608,13 +2613,13 @@
       <c r="F3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="111" t="s">
+      <c r="J3" s="73" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="R3" s="72" t="s">
+      <c r="R3" s="125" t="s">
         <v>15</v>
       </c>
       <c r="S3" s="69" t="s">
@@ -2637,13 +2642,13 @@
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="31"/>
-      <c r="J4" s="112" t="s">
+      <c r="J4" s="74" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="37">
         <v>0.31</v>
       </c>
-      <c r="R4" s="73"/>
+      <c r="R4" s="126"/>
       <c r="S4" s="65" t="s">
         <v>350</v>
       </c>
@@ -2662,13 +2667,13 @@
       <c r="D5" s="13"/>
       <c r="E5" s="16"/>
       <c r="F5" s="31"/>
-      <c r="J5" s="113" t="s">
+      <c r="J5" s="75" t="s">
         <v>61</v>
       </c>
       <c r="K5" s="38">
         <v>0.23</v>
       </c>
-      <c r="R5" s="73"/>
+      <c r="R5" s="126"/>
       <c r="S5" s="65" t="s">
         <v>351</v>
       </c>
@@ -2687,13 +2692,13 @@
       <c r="D6" s="13"/>
       <c r="E6" s="16"/>
       <c r="F6" s="31"/>
-      <c r="J6" s="113" t="s">
+      <c r="J6" s="75" t="s">
         <v>62</v>
       </c>
       <c r="K6" s="38">
         <v>0.16</v>
       </c>
-      <c r="R6" s="73"/>
+      <c r="R6" s="126"/>
       <c r="S6" s="65" t="s">
         <v>352</v>
       </c>
@@ -2712,13 +2717,13 @@
       <c r="D7" s="13"/>
       <c r="E7" s="16"/>
       <c r="F7" s="31"/>
-      <c r="J7" s="113" t="s">
+      <c r="J7" s="75" t="s">
         <v>63</v>
       </c>
       <c r="K7" s="38">
         <v>0.15</v>
       </c>
-      <c r="R7" s="73"/>
+      <c r="R7" s="126"/>
       <c r="S7" s="65" t="s">
         <v>353</v>
       </c>
@@ -2737,13 +2742,13 @@
       <c r="D8" s="13"/>
       <c r="E8" s="16"/>
       <c r="F8" s="31"/>
-      <c r="J8" s="113" t="s">
+      <c r="J8" s="75" t="s">
         <v>64</v>
       </c>
       <c r="K8" s="38">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="R8" s="73"/>
+      <c r="R8" s="126"/>
       <c r="S8" s="65" t="s">
         <v>354</v>
       </c>
@@ -2754,7 +2759,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
@@ -2762,13 +2767,13 @@
       <c r="D9" s="14"/>
       <c r="E9" s="17"/>
       <c r="F9" s="32"/>
-      <c r="J9" s="113" t="s">
+      <c r="J9" s="75" t="s">
         <v>65</v>
       </c>
       <c r="K9" s="45">
         <v>0.04</v>
       </c>
-      <c r="R9" s="73"/>
+      <c r="R9" s="126"/>
       <c r="S9" s="65" t="s">
         <v>355</v>
       </c>
@@ -2784,13 +2789,13 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="33"/>
-      <c r="J10" s="113" t="s">
+      <c r="J10" s="75" t="s">
         <v>67</v>
       </c>
       <c r="K10" s="45">
         <v>0.02</v>
       </c>
-      <c r="R10" s="73"/>
+      <c r="R10" s="126"/>
       <c r="S10" s="65" t="s">
         <v>356</v>
       </c>
@@ -2801,14 +2806,14 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J11" s="114" t="s">
+    <row r="11" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="76" t="s">
         <v>68</v>
       </c>
       <c r="K11" s="43">
         <v>0.02</v>
       </c>
-      <c r="R11" s="74"/>
+      <c r="R11" s="127"/>
       <c r="S11" s="66" t="s">
         <v>357</v>
       </c>
@@ -2824,7 +2829,7 @@
         <f>SUM(K4:K11)</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="R12" s="72" t="s">
+      <c r="R12" s="125" t="s">
         <v>31</v>
       </c>
       <c r="S12" s="69" t="s">
@@ -2837,7 +2842,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="34"/>
       <c r="C13" s="34" t="s">
         <v>35</v>
@@ -2853,7 +2858,7 @@
       <c r="J13" t="s">
         <v>35</v>
       </c>
-      <c r="R13" s="73"/>
+      <c r="R13" s="126"/>
       <c r="S13" s="65" t="s">
         <v>359</v>
       </c>
@@ -2864,28 +2869,28 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="89" t="s">
+    <row r="14" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="72" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="96" t="s">
+      <c r="D14" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="97"/>
+      <c r="E14" s="111"/>
       <c r="F14" s="23" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="34"/>
-      <c r="J14" s="89" t="s">
+      <c r="J14" s="72" t="s">
         <v>7</v>
       </c>
       <c r="K14" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="R14" s="73"/>
+      <c r="R14" s="126"/>
       <c r="S14" s="65" t="s">
         <v>360</v>
       </c>
@@ -2897,27 +2902,27 @@
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="81">
+      <c r="C15" s="99">
         <v>0.1</v>
       </c>
-      <c r="D15" s="98" t="s">
+      <c r="D15" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="99"/>
+      <c r="E15" s="113"/>
       <c r="F15" s="37">
         <v>0.12</v>
       </c>
       <c r="G15" s="34"/>
-      <c r="J15" s="115" t="s">
+      <c r="J15" s="77" t="s">
         <v>70</v>
       </c>
       <c r="K15" s="42">
         <v>0.5</v>
       </c>
-      <c r="R15" s="73"/>
+      <c r="R15" s="126"/>
       <c r="S15" s="65" t="s">
         <v>361</v>
       </c>
@@ -2928,24 +2933,24 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="91"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="100" t="s">
+    <row r="16" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="97"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="101"/>
+      <c r="E16" s="109"/>
       <c r="F16" s="38">
         <v>0.12</v>
       </c>
       <c r="G16" s="34"/>
-      <c r="J16" s="116" t="s">
+      <c r="J16" s="78" t="s">
         <v>71</v>
       </c>
       <c r="K16" s="43">
         <v>0.5</v>
       </c>
-      <c r="R16" s="73"/>
+      <c r="R16" s="126"/>
       <c r="S16" s="65" t="s">
         <v>362</v>
       </c>
@@ -2957,17 +2962,17 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="91"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="100" t="s">
+      <c r="B17" s="97"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="101"/>
+      <c r="E17" s="109"/>
       <c r="F17" s="38">
         <v>0.15</v>
       </c>
       <c r="G17" s="34"/>
-      <c r="R17" s="73"/>
+      <c r="R17" s="126"/>
       <c r="S17" s="65" t="s">
         <v>363</v>
       </c>
@@ -2978,20 +2983,20 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="91"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="100" t="s">
+    <row r="18" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="97"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="101"/>
+      <c r="E18" s="109"/>
       <c r="F18" s="38">
         <v>0.11</v>
       </c>
       <c r="G18" s="34">
         <v>546431</v>
       </c>
-      <c r="R18" s="73"/>
+      <c r="R18" s="126"/>
       <c r="S18" s="65" t="s">
         <v>364</v>
       </c>
@@ -3002,24 +3007,24 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="91"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="100" t="s">
+    <row r="19" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="97"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="101"/>
+      <c r="E19" s="109"/>
       <c r="F19" s="38">
         <v>0.08</v>
       </c>
       <c r="G19" s="34"/>
-      <c r="J19" s="89" t="s">
+      <c r="J19" s="72" t="s">
         <v>8</v>
       </c>
       <c r="K19" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="R19" s="73"/>
+      <c r="R19" s="126"/>
       <c r="S19" s="65" t="s">
         <v>365</v>
       </c>
@@ -3030,24 +3035,24 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="91"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="100" t="s">
+    <row r="20" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="97"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="108" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="101"/>
+      <c r="E20" s="109"/>
       <c r="F20" s="38">
         <v>0.03</v>
       </c>
       <c r="G20" s="34"/>
-      <c r="J20" s="115" t="s">
+      <c r="J20" s="77" t="s">
         <v>88</v>
       </c>
       <c r="K20" s="60">
         <v>0.65</v>
       </c>
-      <c r="R20" s="74"/>
+      <c r="R20" s="127"/>
       <c r="S20" s="66" t="s">
         <v>366</v>
       </c>
@@ -3059,23 +3064,23 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="91"/>
-      <c r="C21" s="78"/>
-      <c r="D21" s="100" t="s">
+      <c r="B21" s="97"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="101"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="38">
         <v>0.03</v>
       </c>
       <c r="G21" s="34"/>
-      <c r="J21" s="117" t="s">
+      <c r="J21" s="79" t="s">
         <v>89</v>
       </c>
       <c r="K21" s="62">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R21" s="72" t="s">
+      <c r="R21" s="125" t="s">
         <v>170</v>
       </c>
       <c r="S21" s="69" t="s">
@@ -3088,24 +3093,24 @@
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="91"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="100" t="s">
+    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="97"/>
+      <c r="C22" s="100"/>
+      <c r="D22" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="101"/>
+      <c r="E22" s="109"/>
       <c r="F22" s="38">
         <v>0.02</v>
       </c>
       <c r="G22" s="34"/>
-      <c r="J22" s="116" t="s">
+      <c r="J22" s="78" t="s">
         <v>90</v>
       </c>
       <c r="K22" s="61">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="R22" s="73"/>
+      <c r="R22" s="126"/>
       <c r="S22" s="65" t="s">
         <v>368</v>
       </c>
@@ -3117,17 +3122,17 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B23" s="91"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="100" t="s">
+      <c r="B23" s="97"/>
+      <c r="C23" s="100"/>
+      <c r="D23" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="101"/>
+      <c r="E23" s="109"/>
       <c r="F23" s="38">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G23" s="34"/>
-      <c r="R23" s="73"/>
+      <c r="R23" s="126"/>
       <c r="S23" s="65" t="s">
         <v>369</v>
       </c>
@@ -3138,18 +3143,18 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="92"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="102" t="s">
+    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="98"/>
+      <c r="C24" s="101"/>
+      <c r="D24" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="103"/>
+      <c r="E24" s="115"/>
       <c r="F24" s="39">
         <v>0.27</v>
       </c>
       <c r="G24" s="34"/>
-      <c r="R24" s="73"/>
+      <c r="R24" s="126"/>
       <c r="S24" s="65" t="s">
         <v>370</v>
       </c>
@@ -3161,21 +3166,21 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="90" t="s">
+      <c r="B25" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="82">
+      <c r="C25" s="102">
         <v>0.13</v>
       </c>
-      <c r="D25" s="98" t="s">
+      <c r="D25" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="99"/>
+      <c r="E25" s="113"/>
       <c r="F25" s="37">
         <v>0.44</v>
       </c>
       <c r="G25" s="34"/>
-      <c r="R25" s="73"/>
+      <c r="R25" s="126"/>
       <c r="S25" s="65" t="s">
         <v>371</v>
       </c>
@@ -3188,17 +3193,17 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
-      <c r="B26" s="91"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="100" t="s">
+      <c r="B26" s="97"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="101"/>
+      <c r="E26" s="109"/>
       <c r="F26" s="38">
         <v>0.17</v>
       </c>
       <c r="G26" s="34"/>
-      <c r="R26" s="73"/>
+      <c r="R26" s="126"/>
       <c r="S26" s="65" t="s">
         <v>372</v>
       </c>
@@ -3209,13 +3214,13 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="91"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="100" t="s">
+    <row r="27" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="97"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="101"/>
+      <c r="E27" s="109"/>
       <c r="F27" s="38">
         <v>0.05</v>
       </c>
@@ -3225,7 +3230,7 @@
       <c r="J27" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="R27" s="73"/>
+      <c r="R27" s="126"/>
       <c r="S27" s="65" t="s">
         <v>373</v>
       </c>
@@ -3236,19 +3241,19 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
-      <c r="B28" s="91"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="100" t="s">
+      <c r="B28" s="97"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="108" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="101"/>
+      <c r="E28" s="109"/>
       <c r="F28" s="38">
         <v>0.28000000000000003</v>
       </c>
       <c r="G28" s="34"/>
-      <c r="J28" s="118" t="s">
+      <c r="J28" s="80" t="s">
         <v>9</v>
       </c>
       <c r="K28" s="21" t="s">
@@ -3257,7 +3262,7 @@
       <c r="L28" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="R28" s="73"/>
+      <c r="R28" s="126"/>
       <c r="S28" s="65" t="s">
         <v>374</v>
       </c>
@@ -3268,18 +3273,18 @@
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="92"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="102" t="s">
+    <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="98"/>
+      <c r="C29" s="104"/>
+      <c r="D29" s="114" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="103"/>
+      <c r="E29" s="115"/>
       <c r="F29" s="39">
         <v>0.06</v>
       </c>
       <c r="G29" s="34"/>
-      <c r="J29" s="119" t="s">
+      <c r="J29" s="81" t="s">
         <v>135</v>
       </c>
       <c r="K29" s="59">
@@ -3288,7 +3293,7 @@
       <c r="L29" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="R29" s="74"/>
+      <c r="R29" s="127"/>
       <c r="S29" s="66" t="s">
         <v>375</v>
       </c>
@@ -3300,21 +3305,21 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="90" t="s">
+      <c r="B30" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="85">
+      <c r="C30" s="105">
         <v>0.59</v>
       </c>
-      <c r="D30" s="98" t="s">
+      <c r="D30" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="99"/>
+      <c r="E30" s="113"/>
       <c r="F30" s="37">
         <v>0.36</v>
       </c>
       <c r="G30" s="34"/>
-      <c r="J30" s="120" t="s">
+      <c r="J30" s="82" t="s">
         <v>136</v>
       </c>
       <c r="K30" s="57">
@@ -3323,7 +3328,7 @@
       <c r="L30" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="R30" s="72" t="s">
+      <c r="R30" s="125" t="s">
         <v>207</v>
       </c>
       <c r="S30" s="69" t="s">
@@ -3337,17 +3342,17 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B31" s="91"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="100" t="s">
+      <c r="B31" s="97"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="108" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="101"/>
+      <c r="E31" s="109"/>
       <c r="F31" s="38">
         <v>0.03</v>
       </c>
       <c r="G31" s="34"/>
-      <c r="J31" s="120" t="s">
+      <c r="J31" s="82" t="s">
         <v>137</v>
       </c>
       <c r="K31" s="57">
@@ -3356,7 +3361,7 @@
       <c r="L31" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="R31" s="73"/>
+      <c r="R31" s="126"/>
       <c r="S31" s="65" t="s">
         <v>377</v>
       </c>
@@ -3368,17 +3373,17 @@
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B32" s="91"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="100" t="s">
+      <c r="B32" s="97"/>
+      <c r="C32" s="106"/>
+      <c r="D32" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="101"/>
+      <c r="E32" s="109"/>
       <c r="F32" s="38">
         <v>0.03</v>
       </c>
       <c r="G32" s="34"/>
-      <c r="J32" s="120" t="s">
+      <c r="J32" s="82" t="s">
         <v>138</v>
       </c>
       <c r="K32" s="57">
@@ -3387,7 +3392,7 @@
       <c r="L32" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="R32" s="73"/>
+      <c r="R32" s="126"/>
       <c r="S32" s="65" t="s">
         <v>378</v>
       </c>
@@ -3399,17 +3404,17 @@
       </c>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B33" s="91"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="100" t="s">
+      <c r="B33" s="97"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="101"/>
+      <c r="E33" s="109"/>
       <c r="F33" s="38">
         <v>0.01</v>
       </c>
       <c r="G33" s="34"/>
-      <c r="J33" s="120" t="s">
+      <c r="J33" s="82" t="s">
         <v>139</v>
       </c>
       <c r="K33" s="57">
@@ -3418,7 +3423,7 @@
       <c r="L33" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="R33" s="73"/>
+      <c r="R33" s="126"/>
       <c r="S33" s="65" t="s">
         <v>379</v>
       </c>
@@ -3429,18 +3434,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="34" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="91"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="100" t="s">
+    <row r="34" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="97"/>
+      <c r="C34" s="106"/>
+      <c r="D34" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="101"/>
+      <c r="E34" s="109"/>
       <c r="F34" s="38">
         <v>0.34</v>
       </c>
       <c r="G34" s="34"/>
-      <c r="J34" s="121" t="s">
+      <c r="J34" s="83" t="s">
         <v>140</v>
       </c>
       <c r="K34" s="58">
@@ -3449,7 +3454,7 @@
       <c r="L34" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="R34" s="73"/>
+      <c r="R34" s="126"/>
       <c r="S34" s="65" t="s">
         <v>380</v>
       </c>
@@ -3461,19 +3466,19 @@
       </c>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B35" s="91"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="100" t="s">
+      <c r="B35" s="97"/>
+      <c r="C35" s="106"/>
+      <c r="D35" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="101"/>
+      <c r="E35" s="109"/>
       <c r="F35" s="38">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G35" s="35">
         <v>3952335</v>
       </c>
-      <c r="R35" s="73"/>
+      <c r="R35" s="126"/>
       <c r="S35" s="65" t="s">
         <v>381</v>
       </c>
@@ -3484,18 +3489,18 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="91"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="100" t="s">
+    <row r="36" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="97"/>
+      <c r="C36" s="106"/>
+      <c r="D36" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="101"/>
+      <c r="E36" s="109"/>
       <c r="F36" s="38">
         <v>0.03</v>
       </c>
       <c r="G36" s="34"/>
-      <c r="R36" s="73"/>
+      <c r="R36" s="126"/>
       <c r="S36" s="65" t="s">
         <v>382</v>
       </c>
@@ -3506,24 +3511,24 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="91"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="100" t="s">
+    <row r="37" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="97"/>
+      <c r="C37" s="106"/>
+      <c r="D37" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="101"/>
+      <c r="E37" s="109"/>
       <c r="F37" s="38">
         <v>0.05</v>
       </c>
       <c r="G37" s="34"/>
-      <c r="J37" s="89" t="s">
+      <c r="J37" s="72" t="s">
         <v>10</v>
       </c>
       <c r="K37" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="R37" s="73"/>
+      <c r="R37" s="126"/>
       <c r="S37" s="65" t="s">
         <v>383</v>
       </c>
@@ -3534,24 +3539,24 @@
         <v>205</v>
       </c>
     </row>
-    <row r="38" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="91"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="100" t="s">
+    <row r="38" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="97"/>
+      <c r="C38" s="106"/>
+      <c r="D38" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="101"/>
+      <c r="E38" s="109"/>
       <c r="F38" s="38">
         <v>0.04</v>
       </c>
       <c r="G38" s="34"/>
-      <c r="J38" s="115" t="s">
+      <c r="J38" s="77" t="s">
         <v>91</v>
       </c>
       <c r="K38" s="60">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R38" s="74"/>
+      <c r="R38" s="127"/>
       <c r="S38" s="66" t="s">
         <v>384</v>
       </c>
@@ -3563,23 +3568,23 @@
       </c>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B39" s="91"/>
-      <c r="C39" s="86"/>
-      <c r="D39" s="100" t="s">
+      <c r="B39" s="97"/>
+      <c r="C39" s="106"/>
+      <c r="D39" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="101"/>
+      <c r="E39" s="109"/>
       <c r="F39" s="38">
         <v>0.02</v>
       </c>
       <c r="G39" s="34"/>
-      <c r="J39" s="117" t="s">
+      <c r="J39" s="79" t="s">
         <v>92</v>
       </c>
       <c r="K39" s="62">
         <v>0.27</v>
       </c>
-      <c r="R39" s="72" t="s">
+      <c r="R39" s="125" t="s">
         <v>33</v>
       </c>
       <c r="S39" s="69" t="s">
@@ -3592,24 +3597,24 @@
         <v>217</v>
       </c>
     </row>
-    <row r="40" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="92"/>
-      <c r="C40" s="87"/>
-      <c r="D40" s="102" t="s">
+    <row r="40" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="98"/>
+      <c r="C40" s="107"/>
+      <c r="D40" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="103"/>
+      <c r="E40" s="115"/>
       <c r="F40" s="39">
         <v>0.02</v>
       </c>
       <c r="G40" s="34"/>
-      <c r="J40" s="117" t="s">
+      <c r="J40" s="79" t="s">
         <v>93</v>
       </c>
       <c r="K40" s="62">
         <v>0.15</v>
       </c>
-      <c r="R40" s="73"/>
+      <c r="R40" s="126"/>
       <c r="S40" s="65" t="s">
         <v>386</v>
       </c>
@@ -3621,27 +3626,27 @@
       </c>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B41" s="93" t="s">
+      <c r="B41" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="75">
+      <c r="C41" s="118">
         <v>0.17</v>
       </c>
-      <c r="D41" s="98" t="s">
+      <c r="D41" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="99"/>
+      <c r="E41" s="113"/>
       <c r="F41" s="37">
         <v>0.16</v>
       </c>
       <c r="G41" s="34"/>
-      <c r="J41" s="117" t="s">
+      <c r="J41" s="79" t="s">
         <v>94</v>
       </c>
       <c r="K41" s="62">
         <v>0.2</v>
       </c>
-      <c r="R41" s="73"/>
+      <c r="R41" s="126"/>
       <c r="S41" s="65" t="s">
         <v>387</v>
       </c>
@@ -3652,24 +3657,24 @@
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="94"/>
-      <c r="C42" s="76"/>
-      <c r="D42" s="100" t="s">
+    <row r="42" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="122"/>
+      <c r="C42" s="119"/>
+      <c r="D42" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="E42" s="101"/>
+      <c r="E42" s="109"/>
       <c r="F42" s="38">
         <v>0.13</v>
       </c>
       <c r="G42" s="34"/>
-      <c r="J42" s="116" t="s">
+      <c r="J42" s="78" t="s">
         <v>95</v>
       </c>
       <c r="K42" s="61">
         <v>0.1</v>
       </c>
-      <c r="R42" s="73"/>
+      <c r="R42" s="126"/>
       <c r="S42" s="65" t="s">
         <v>388</v>
       </c>
@@ -3681,12 +3686,12 @@
       </c>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B43" s="94"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="100" t="s">
+      <c r="B43" s="122"/>
+      <c r="C43" s="119"/>
+      <c r="D43" s="108" t="s">
         <v>48</v>
       </c>
-      <c r="E43" s="101"/>
+      <c r="E43" s="109"/>
       <c r="F43" s="38">
         <v>0.15</v>
       </c>
@@ -3696,7 +3701,7 @@
         <f>SUM(K38:K42)</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="R43" s="73"/>
+      <c r="R43" s="126"/>
       <c r="S43" s="65" t="s">
         <v>389</v>
       </c>
@@ -3707,18 +3712,18 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="94"/>
-      <c r="C44" s="76"/>
-      <c r="D44" s="100" t="s">
+    <row r="44" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="122"/>
+      <c r="C44" s="119"/>
+      <c r="D44" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="E44" s="101"/>
+      <c r="E44" s="109"/>
       <c r="F44" s="38">
         <v>0.28999999999999998</v>
       </c>
       <c r="G44" s="34"/>
-      <c r="R44" s="73"/>
+      <c r="R44" s="126"/>
       <c r="S44" s="65" t="s">
         <v>390</v>
       </c>
@@ -3729,26 +3734,26 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="94"/>
-      <c r="C45" s="76"/>
-      <c r="D45" s="100" t="s">
+    <row r="45" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="122"/>
+      <c r="C45" s="119"/>
+      <c r="D45" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="E45" s="101"/>
+      <c r="E45" s="109"/>
       <c r="F45" s="38">
         <v>0.05</v>
       </c>
       <c r="G45" s="34">
         <v>668392</v>
       </c>
-      <c r="J45" s="122" t="s">
+      <c r="J45" s="84" t="s">
         <v>11</v>
       </c>
       <c r="K45" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="R45" s="73"/>
+      <c r="R45" s="126"/>
       <c r="S45" s="65" t="s">
         <v>391</v>
       </c>
@@ -3759,24 +3764,24 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="94"/>
-      <c r="C46" s="76"/>
-      <c r="D46" s="100" t="s">
+    <row r="46" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="122"/>
+      <c r="C46" s="119"/>
+      <c r="D46" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="101"/>
+      <c r="E46" s="109"/>
       <c r="F46" s="38">
         <v>0.06</v>
       </c>
       <c r="G46" s="34"/>
-      <c r="J46" s="122" t="s">
+      <c r="J46" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="K46" s="123">
+      <c r="K46" s="85">
         <v>0.15</v>
       </c>
-      <c r="R46" s="73"/>
+      <c r="R46" s="126"/>
       <c r="S46" s="65" t="s">
         <v>392</v>
       </c>
@@ -3787,20 +3792,20 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="94"/>
-      <c r="C47" s="76"/>
-      <c r="D47" s="100" t="s">
+    <row r="47" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="122"/>
+      <c r="C47" s="119"/>
+      <c r="D47" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="E47" s="101"/>
+      <c r="E47" s="109"/>
       <c r="F47" s="38">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G47" s="34"/>
       <c r="J47" s="34"/>
       <c r="K47" s="34"/>
-      <c r="R47" s="74"/>
+      <c r="R47" s="127"/>
       <c r="S47" s="66" t="s">
         <v>209</v>
       </c>
@@ -3811,20 +3816,20 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="95"/>
-      <c r="C48" s="77"/>
-      <c r="D48" s="95" t="s">
+    <row r="48" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="123"/>
+      <c r="C48" s="120"/>
+      <c r="D48" s="123" t="s">
         <v>59</v>
       </c>
-      <c r="E48" s="104"/>
+      <c r="E48" s="124"/>
       <c r="F48" s="39">
         <v>0.09</v>
       </c>
       <c r="G48" s="34"/>
       <c r="J48" s="34"/>
       <c r="K48" s="34"/>
-      <c r="R48" s="72" t="s">
+      <c r="R48" s="125" t="s">
         <v>225</v>
       </c>
       <c r="S48" s="69" t="s">
@@ -3837,26 +3842,26 @@
         <v>235</v>
       </c>
     </row>
-    <row r="49" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="90" t="s">
+    <row r="49" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C49" s="75">
+      <c r="C49" s="118">
         <v>0.01</v>
       </c>
-      <c r="D49" s="105" t="s">
+      <c r="D49" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="106"/>
+      <c r="E49" s="117"/>
       <c r="F49" s="37">
         <v>0.66</v>
       </c>
       <c r="G49" s="34"/>
-      <c r="J49" s="80" t="s">
+      <c r="J49" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="K49" s="80"/>
-      <c r="R49" s="73"/>
+      <c r="K49" s="91"/>
+      <c r="R49" s="126"/>
       <c r="S49" s="65" t="s">
         <v>394</v>
       </c>
@@ -3867,23 +3872,23 @@
         <v>236</v>
       </c>
     </row>
-    <row r="50" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="91"/>
-      <c r="C50" s="76"/>
-      <c r="D50" s="107" t="s">
+    <row r="50" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="97"/>
+      <c r="C50" s="119"/>
+      <c r="D50" s="128" t="s">
         <v>55</v>
       </c>
-      <c r="E50" s="108"/>
+      <c r="E50" s="129"/>
       <c r="F50" s="38">
         <v>0.21</v>
       </c>
       <c r="G50" s="34">
         <v>37707</v>
       </c>
-      <c r="J50" s="124" t="s">
+      <c r="J50" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="K50" s="125"/>
+      <c r="K50" s="93"/>
       <c r="L50" s="41" t="s">
         <v>77</v>
       </c>
@@ -3896,7 +3901,7 @@
       <c r="O50" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="R50" s="73"/>
+      <c r="R50" s="126"/>
       <c r="S50" s="65" t="s">
         <v>395</v>
       </c>
@@ -3907,21 +3912,21 @@
         <v>237</v>
       </c>
     </row>
-    <row r="51" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="92"/>
-      <c r="C51" s="77"/>
-      <c r="D51" s="109" t="s">
+    <row r="51" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="98"/>
+      <c r="C51" s="120"/>
+      <c r="D51" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="E51" s="110"/>
+      <c r="E51" s="131"/>
       <c r="F51" s="40">
         <v>0.13</v>
       </c>
       <c r="G51" s="34"/>
-      <c r="J51" s="126" t="s">
+      <c r="J51" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="K51" s="127"/>
+      <c r="K51" s="95"/>
       <c r="L51" s="46">
         <v>0.15</v>
       </c>
@@ -3935,7 +3940,7 @@
       <c r="O51" s="27">
         <v>541</v>
       </c>
-      <c r="R51" s="73"/>
+      <c r="R51" s="126"/>
       <c r="S51" s="65" t="s">
         <v>396</v>
       </c>
@@ -3947,10 +3952,10 @@
       </c>
     </row>
     <row r="52" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J52" s="128" t="s">
+      <c r="J52" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="K52" s="129"/>
+      <c r="K52" s="87"/>
       <c r="L52" s="47">
         <f>N52/N86</f>
         <v>3.4018574559115097E-2</v>
@@ -3965,7 +3970,7 @@
       <c r="O52" s="25">
         <v>317</v>
       </c>
-      <c r="R52" s="73"/>
+      <c r="R52" s="126"/>
       <c r="S52" s="65" t="s">
         <v>397</v>
       </c>
@@ -3977,10 +3982,10 @@
       </c>
     </row>
     <row r="53" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J53" s="128" t="s">
+      <c r="J53" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="K53" s="129"/>
+      <c r="K53" s="87"/>
       <c r="L53" s="47">
         <f>N53/N86</f>
         <v>5.9480329750600022E-3</v>
@@ -3994,7 +3999,7 @@
       <c r="O53" s="25">
         <v>35</v>
       </c>
-      <c r="R53" s="73"/>
+      <c r="R53" s="126"/>
       <c r="S53" s="65" t="s">
         <v>398</v>
       </c>
@@ -4006,10 +4011,10 @@
       </c>
     </row>
     <row r="54" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J54" s="128" t="s">
+      <c r="J54" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="K54" s="129"/>
+      <c r="K54" s="87"/>
       <c r="L54" s="47">
         <f>N54/N86</f>
         <v>3.7253469685902117E-2</v>
@@ -4024,7 +4029,7 @@
       <c r="O54" s="25">
         <v>209</v>
       </c>
-      <c r="R54" s="73"/>
+      <c r="R54" s="126"/>
       <c r="S54" s="65" t="s">
         <v>399</v>
       </c>
@@ -4042,10 +4047,10 @@
       <c r="C55" t="s">
         <v>78</v>
       </c>
-      <c r="J55" s="128" t="s">
+      <c r="J55" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="K55" s="129"/>
+      <c r="K55" s="87"/>
       <c r="L55" s="47">
         <f>N55/N86</f>
         <v>7.9307106334133362E-3</v>
@@ -4060,7 +4065,7 @@
       <c r="O55" s="25">
         <v>153</v>
       </c>
-      <c r="R55" s="73"/>
+      <c r="R55" s="126"/>
       <c r="S55" s="65" t="s">
         <v>400</v>
       </c>
@@ -4071,14 +4076,14 @@
         <v>242</v>
       </c>
     </row>
-    <row r="56" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>79</v>
       </c>
-      <c r="J56" s="128" t="s">
+      <c r="J56" s="86" t="s">
         <v>105</v>
       </c>
-      <c r="K56" s="129"/>
+      <c r="K56" s="87"/>
       <c r="L56" s="47">
         <f>N56/N86</f>
         <v>1.6591881456746321E-2</v>
@@ -4093,7 +4098,7 @@
       <c r="O56" s="25">
         <v>139</v>
       </c>
-      <c r="R56" s="74"/>
+      <c r="R56" s="127"/>
       <c r="S56" s="66" t="s">
         <v>401</v>
       </c>
@@ -4108,10 +4113,10 @@
       <c r="B57" t="s">
         <v>80</v>
       </c>
-      <c r="J57" s="128" t="s">
+      <c r="J57" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="K57" s="129"/>
+      <c r="K57" s="87"/>
       <c r="L57" s="47">
         <f>N57/N86</f>
         <v>1.168736303871439E-2</v>
@@ -4125,7 +4130,7 @@
       <c r="O57" s="25">
         <v>43</v>
       </c>
-      <c r="R57" s="72" t="s">
+      <c r="R57" s="125" t="s">
         <v>51</v>
       </c>
       <c r="S57" s="69" t="s">
@@ -4142,10 +4147,10 @@
       <c r="B58" t="s">
         <v>81</v>
       </c>
-      <c r="J58" s="128" t="s">
+      <c r="J58" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="K58" s="129"/>
+      <c r="K58" s="87"/>
       <c r="L58" s="47">
         <f>N58/N86</f>
         <v>1.7322341646665972E-2</v>
@@ -4160,7 +4165,7 @@
       <c r="O58" s="25">
         <v>147</v>
       </c>
-      <c r="R58" s="73"/>
+      <c r="R58" s="126"/>
       <c r="S58" s="65" t="s">
         <v>429</v>
       </c>
@@ -4175,10 +4180,10 @@
       <c r="B59" t="s">
         <v>82</v>
       </c>
-      <c r="J59" s="128" t="s">
+      <c r="J59" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="K59" s="129"/>
+      <c r="K59" s="87"/>
       <c r="L59" s="47">
         <f>N59/N86</f>
         <v>4.1844933736825629E-2</v>
@@ -4193,7 +4198,7 @@
       <c r="O59" s="25">
         <v>223</v>
       </c>
-      <c r="R59" s="73"/>
+      <c r="R59" s="126"/>
       <c r="S59" s="65" t="s">
         <v>430</v>
       </c>
@@ -4205,10 +4210,10 @@
       </c>
     </row>
     <row r="60" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J60" s="128" t="s">
+      <c r="J60" s="86" t="s">
         <v>109</v>
       </c>
-      <c r="K60" s="129"/>
+      <c r="K60" s="87"/>
       <c r="L60" s="47">
         <f>N60/N86</f>
         <v>1.5548366899718251E-2</v>
@@ -4223,7 +4228,7 @@
       <c r="O60" s="25">
         <v>65</v>
       </c>
-      <c r="R60" s="73"/>
+      <c r="R60" s="126"/>
       <c r="S60" s="65" t="s">
         <v>431</v>
       </c>
@@ -4238,10 +4243,10 @@
       <c r="B61" t="s">
         <v>83</v>
       </c>
-      <c r="J61" s="128" t="s">
+      <c r="J61" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K61" s="129"/>
+      <c r="K61" s="87"/>
       <c r="L61" s="47">
         <f>N61/N86</f>
         <v>9.7046853803610562E-3</v>
@@ -4256,7 +4261,7 @@
       <c r="O61" s="25">
         <v>97</v>
       </c>
-      <c r="R61" s="73"/>
+      <c r="R61" s="126"/>
       <c r="S61" s="65" t="s">
         <v>432</v>
       </c>
@@ -4271,10 +4276,10 @@
       <c r="B62" t="s">
         <v>84</v>
       </c>
-      <c r="J62" s="128" t="s">
+      <c r="J62" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="K62" s="129"/>
+      <c r="K62" s="87"/>
       <c r="L62" s="47">
         <f>N62/N86</f>
         <v>2.1600751330481061E-2</v>
@@ -4289,7 +4294,7 @@
       <c r="O62" s="25">
         <v>208</v>
       </c>
-      <c r="R62" s="73"/>
+      <c r="R62" s="126"/>
       <c r="S62" s="65" t="s">
         <v>433</v>
       </c>
@@ -4304,10 +4309,10 @@
       <c r="B63" t="s">
         <v>85</v>
       </c>
-      <c r="J63" s="128" t="s">
+      <c r="J63" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="K63" s="129"/>
+      <c r="K63" s="87"/>
       <c r="L63" s="47">
         <f>N63/N86</f>
         <v>1.095690284879474E-2</v>
@@ -4322,7 +4327,7 @@
       <c r="O63" s="25">
         <v>252</v>
       </c>
-      <c r="R63" s="73"/>
+      <c r="R63" s="126"/>
       <c r="S63" s="65" t="s">
         <v>434</v>
       </c>
@@ -4337,10 +4342,10 @@
       <c r="B64" t="s">
         <v>86</v>
       </c>
-      <c r="J64" s="128" t="s">
+      <c r="J64" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="K64" s="129"/>
+      <c r="K64" s="87"/>
       <c r="L64" s="47">
         <f>N64/N86</f>
         <v>3.8714390065741421E-2</v>
@@ -4355,7 +4360,7 @@
       <c r="O64" s="25">
         <v>436</v>
       </c>
-      <c r="R64" s="73"/>
+      <c r="R64" s="126"/>
       <c r="S64" s="65" t="s">
         <v>435</v>
       </c>
@@ -4366,14 +4371,14 @@
         <v>260</v>
       </c>
     </row>
-    <row r="65" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>87</v>
       </c>
-      <c r="J65" s="128" t="s">
+      <c r="J65" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="K65" s="129"/>
+      <c r="K65" s="87"/>
       <c r="L65" s="47">
         <f>N65/N86</f>
         <v>6.9185015130961078E-2</v>
@@ -4387,7 +4392,7 @@
       <c r="O65" s="25">
         <v>750</v>
       </c>
-      <c r="R65" s="74"/>
+      <c r="R65" s="127"/>
       <c r="S65" s="66" t="s">
         <v>436</v>
       </c>
@@ -4399,10 +4404,10 @@
       </c>
     </row>
     <row r="66" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J66" s="128" t="s">
+      <c r="J66" s="86" t="s">
         <v>115</v>
       </c>
-      <c r="K66" s="129"/>
+      <c r="K66" s="87"/>
       <c r="L66" s="47">
         <f>N66/N86</f>
         <v>1.6487530001043516E-2</v>
@@ -4417,7 +4422,7 @@
       <c r="O66" s="25">
         <v>126</v>
       </c>
-      <c r="R66" s="72" t="s">
+      <c r="R66" s="125" t="s">
         <v>19</v>
       </c>
       <c r="S66" s="69" t="s">
@@ -4431,10 +4436,10 @@
       </c>
     </row>
     <row r="67" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J67" s="128" t="s">
+      <c r="J67" s="86" t="s">
         <v>116</v>
       </c>
-      <c r="K67" s="129"/>
+      <c r="K67" s="87"/>
       <c r="L67" s="47">
         <f>N67/N86</f>
         <v>6.1880413231764582E-2</v>
@@ -4449,7 +4454,7 @@
       <c r="O67" s="25">
         <v>434</v>
       </c>
-      <c r="R67" s="73"/>
+      <c r="R67" s="126"/>
       <c r="S67" s="65" t="s">
         <v>403</v>
       </c>
@@ -4464,10 +4469,10 @@
       <c r="B68" t="s">
         <v>439</v>
       </c>
-      <c r="J68" s="128" t="s">
+      <c r="J68" s="86" t="s">
         <v>117</v>
       </c>
-      <c r="K68" s="129"/>
+      <c r="K68" s="87"/>
       <c r="L68" s="47">
         <f>N68/N86</f>
         <v>3.4749034749034749E-2</v>
@@ -4482,7 +4487,7 @@
       <c r="O68" s="25">
         <v>334</v>
       </c>
-      <c r="R68" s="73"/>
+      <c r="R68" s="126"/>
       <c r="S68" s="65" t="s">
         <v>404</v>
       </c>
@@ -4494,10 +4499,10 @@
       </c>
     </row>
     <row r="69" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J69" s="128" t="s">
+      <c r="J69" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="K69" s="129"/>
+      <c r="K69" s="87"/>
       <c r="L69" s="47">
         <f>N69/N86</f>
         <v>5.1132213294375461E-3</v>
@@ -4512,7 +4517,7 @@
       <c r="O69" s="25">
         <v>354</v>
       </c>
-      <c r="R69" s="73"/>
+      <c r="R69" s="126"/>
       <c r="S69" s="65" t="s">
         <v>405</v>
       </c>
@@ -4524,10 +4529,10 @@
       </c>
     </row>
     <row r="70" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J70" s="128" t="s">
+      <c r="J70" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="K70" s="129"/>
+      <c r="K70" s="87"/>
       <c r="L70" s="47">
         <f>N70/N86</f>
         <v>1.3983095064176145E-2</v>
@@ -4542,7 +4547,7 @@
       <c r="O70" s="25">
         <v>368</v>
       </c>
-      <c r="R70" s="73"/>
+      <c r="R70" s="126"/>
       <c r="S70" s="65" t="s">
         <v>406</v>
       </c>
@@ -4554,10 +4559,10 @@
       </c>
     </row>
     <row r="71" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J71" s="128" t="s">
+      <c r="J71" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="K71" s="129"/>
+      <c r="K71" s="87"/>
       <c r="L71" s="47">
         <v>0.01</v>
       </c>
@@ -4571,7 +4576,7 @@
       <c r="O71" s="25">
         <v>93</v>
       </c>
-      <c r="R71" s="73"/>
+      <c r="R71" s="126"/>
       <c r="S71" s="65" t="s">
         <v>407</v>
       </c>
@@ -4583,10 +4588,10 @@
       </c>
     </row>
     <row r="72" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J72" s="128" t="s">
+      <c r="J72" s="86" t="s">
         <v>121</v>
       </c>
-      <c r="K72" s="129"/>
+      <c r="K72" s="87"/>
       <c r="L72" s="47">
         <f>N72/N86</f>
         <v>1.3565689241364916E-2</v>
@@ -4601,7 +4606,7 @@
       <c r="O72" s="25">
         <v>120</v>
       </c>
-      <c r="R72" s="73"/>
+      <c r="R72" s="126"/>
       <c r="S72" s="65" t="s">
         <v>408</v>
       </c>
@@ -4613,10 +4618,10 @@
       </c>
     </row>
     <row r="73" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J73" s="128" t="s">
+      <c r="J73" s="86" t="s">
         <v>122</v>
       </c>
-      <c r="K73" s="129"/>
+      <c r="K73" s="87"/>
       <c r="L73" s="47">
         <f>N73/N86</f>
         <v>1.1165605760200354E-2</v>
@@ -4631,7 +4636,7 @@
       <c r="O73" s="25">
         <v>142</v>
       </c>
-      <c r="R73" s="73"/>
+      <c r="R73" s="126"/>
       <c r="S73" s="65" t="s">
         <v>354</v>
       </c>
@@ -4642,11 +4647,11 @@
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J74" s="128" t="s">
+    <row r="74" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J74" s="86" t="s">
         <v>123</v>
       </c>
-      <c r="K74" s="129"/>
+      <c r="K74" s="87"/>
       <c r="L74" s="47">
         <f>N74/N86</f>
         <v>1.0435145570280706E-2</v>
@@ -4661,7 +4666,7 @@
       <c r="O74" s="25">
         <v>128</v>
       </c>
-      <c r="R74" s="74"/>
+      <c r="R74" s="127"/>
       <c r="S74" s="66" t="s">
         <v>409</v>
       </c>
@@ -4673,10 +4678,10 @@
       </c>
     </row>
     <row r="75" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J75" s="128" t="s">
+      <c r="J75" s="86" t="s">
         <v>124</v>
       </c>
-      <c r="K75" s="129"/>
+      <c r="K75" s="87"/>
       <c r="L75" s="47">
         <f>N75/N86</f>
         <v>1.0852551393091934E-2</v>
@@ -4691,7 +4696,7 @@
       <c r="O75" s="25">
         <v>197</v>
       </c>
-      <c r="R75" s="72" t="s">
+      <c r="R75" s="125" t="s">
         <v>49</v>
       </c>
       <c r="S75" s="64" t="s">
@@ -4705,10 +4710,10 @@
       </c>
     </row>
     <row r="76" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J76" s="128" t="s">
+      <c r="J76" s="86" t="s">
         <v>125</v>
       </c>
-      <c r="K76" s="129"/>
+      <c r="K76" s="87"/>
       <c r="L76" s="47">
         <f>N76/N86</f>
         <v>7.1898152979234062E-2</v>
@@ -4723,7 +4728,7 @@
       <c r="O76" s="25">
         <v>829</v>
       </c>
-      <c r="R76" s="73"/>
+      <c r="R76" s="126"/>
       <c r="S76" s="65" t="s">
         <v>420</v>
       </c>
@@ -4735,10 +4740,10 @@
       </c>
     </row>
     <row r="77" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J77" s="128" t="s">
+      <c r="J77" s="86" t="s">
         <v>126</v>
       </c>
-      <c r="K77" s="129"/>
+      <c r="K77" s="87"/>
       <c r="L77" s="47">
         <f>N77/N86</f>
         <v>2.0870291140561412E-2</v>
@@ -4753,7 +4758,7 @@
       <c r="O77" s="25">
         <v>143</v>
       </c>
-      <c r="R77" s="73"/>
+      <c r="R77" s="126"/>
       <c r="S77" s="65" t="s">
         <v>421</v>
       </c>
@@ -4765,10 +4770,10 @@
       </c>
     </row>
     <row r="78" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J78" s="128" t="s">
+      <c r="J78" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="K78" s="129"/>
+      <c r="K78" s="87"/>
       <c r="L78" s="47">
         <f>N78/N86</f>
         <v>2.7340081394135449E-2</v>
@@ -4783,7 +4788,7 @@
       <c r="O78" s="25">
         <v>351</v>
       </c>
-      <c r="R78" s="73"/>
+      <c r="R78" s="126"/>
       <c r="S78" s="65" t="s">
         <v>422</v>
       </c>
@@ -4795,10 +4800,10 @@
       </c>
     </row>
     <row r="79" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J79" s="128" t="s">
+      <c r="J79" s="86" t="s">
         <v>128</v>
       </c>
-      <c r="K79" s="129"/>
+      <c r="K79" s="87"/>
       <c r="L79" s="47">
         <f>N79/N86</f>
         <v>1.6487530001043516E-2</v>
@@ -4813,7 +4818,7 @@
       <c r="O79" s="25">
         <v>229</v>
       </c>
-      <c r="R79" s="73"/>
+      <c r="R79" s="126"/>
       <c r="S79" s="65" t="s">
         <v>423</v>
       </c>
@@ -4825,10 +4830,10 @@
       </c>
     </row>
     <row r="80" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="J80" s="128" t="s">
+      <c r="J80" s="86" t="s">
         <v>129</v>
       </c>
-      <c r="K80" s="129"/>
+      <c r="K80" s="87"/>
       <c r="L80" s="47">
         <f>N80/N86</f>
         <v>1.7426693102368777E-2</v>
@@ -4843,7 +4848,7 @@
       <c r="O80" s="25">
         <v>379</v>
       </c>
-      <c r="R80" s="73"/>
+      <c r="R80" s="126"/>
       <c r="S80" s="65" t="s">
         <v>424</v>
       </c>
@@ -4855,10 +4860,10 @@
       </c>
     </row>
     <row r="81" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="J81" s="128" t="s">
+      <c r="J81" s="86" t="s">
         <v>130</v>
       </c>
-      <c r="K81" s="129"/>
+      <c r="K81" s="87"/>
       <c r="L81" s="47">
         <f>N81/N86</f>
         <v>3.7044766774496501E-2</v>
@@ -4873,7 +4878,7 @@
       <c r="O81" s="25">
         <v>543</v>
       </c>
-      <c r="R81" s="73"/>
+      <c r="R81" s="126"/>
       <c r="S81" s="65" t="s">
         <v>425</v>
       </c>
@@ -4885,10 +4890,10 @@
       </c>
     </row>
     <row r="82" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="J82" s="128" t="s">
+      <c r="J82" s="86" t="s">
         <v>131</v>
       </c>
-      <c r="K82" s="129"/>
+      <c r="K82" s="87"/>
       <c r="L82" s="47">
         <f>N82/N86</f>
         <v>2.1705102786183868E-2</v>
@@ -4903,7 +4908,7 @@
       <c r="O82" s="25">
         <v>381</v>
       </c>
-      <c r="R82" s="73"/>
+      <c r="R82" s="126"/>
       <c r="S82" s="65" t="s">
         <v>426</v>
       </c>
@@ -4914,11 +4919,11 @@
         <v>296</v>
       </c>
     </row>
-    <row r="83" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J83" s="128" t="s">
+    <row r="83" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J83" s="86" t="s">
         <v>132</v>
       </c>
-      <c r="K83" s="129"/>
+      <c r="K83" s="87"/>
       <c r="L83" s="47">
         <v>0.09</v>
       </c>
@@ -4931,7 +4936,7 @@
       <c r="O83" s="25">
         <v>1042</v>
       </c>
-      <c r="R83" s="74"/>
+      <c r="R83" s="127"/>
       <c r="S83" s="71" t="s">
         <v>427</v>
       </c>
@@ -4943,10 +4948,10 @@
       </c>
     </row>
     <row r="84" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="J84" s="128" t="s">
+      <c r="J84" s="86" t="s">
         <v>133</v>
       </c>
-      <c r="K84" s="129"/>
+      <c r="K84" s="87"/>
       <c r="L84" s="47">
         <v>0.01</v>
       </c>
@@ -4959,7 +4964,7 @@
       <c r="O84" s="25">
         <v>10</v>
       </c>
-      <c r="R84" s="72" t="s">
+      <c r="R84" s="125" t="s">
         <v>34</v>
       </c>
       <c r="S84" s="69" t="s">
@@ -4972,11 +4977,11 @@
         <v>321</v>
       </c>
     </row>
-    <row r="85" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J85" s="130" t="s">
+    <row r="85" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J85" s="88" t="s">
         <v>134</v>
       </c>
-      <c r="K85" s="131"/>
+      <c r="K85" s="89"/>
       <c r="L85" s="50">
         <v>0.01</v>
       </c>
@@ -4989,7 +4994,7 @@
       <c r="O85" s="53">
         <v>18</v>
       </c>
-      <c r="R85" s="73"/>
+      <c r="R85" s="126"/>
       <c r="S85" s="65"/>
       <c r="T85" s="26" t="s">
         <v>313</v>
@@ -4998,9 +5003,9 @@
         <v>322</v>
       </c>
     </row>
-    <row r="86" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J86" s="88"/>
-      <c r="K86" s="88"/>
+    <row r="86" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J86" s="90"/>
+      <c r="K86" s="90"/>
       <c r="L86" s="54">
         <f>SUM(L51:L85)</f>
         <v>0.9993123239069186</v>
@@ -5017,7 +5022,7 @@
         <f>SUM(O51:O85)</f>
         <v>9836</v>
       </c>
-      <c r="R86" s="73"/>
+      <c r="R86" s="126"/>
       <c r="S86" s="65"/>
       <c r="T86" s="26" t="s">
         <v>314</v>
@@ -5027,7 +5032,7 @@
       </c>
     </row>
     <row r="87" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="R87" s="73"/>
+      <c r="R87" s="126"/>
       <c r="S87" s="65"/>
       <c r="T87" s="26" t="s">
         <v>315</v>
@@ -5037,7 +5042,7 @@
       </c>
     </row>
     <row r="88" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="R88" s="73"/>
+      <c r="R88" s="126"/>
       <c r="S88" s="65"/>
       <c r="T88" s="26" t="s">
         <v>316</v>
@@ -5047,7 +5052,7 @@
       </c>
     </row>
     <row r="89" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="R89" s="73"/>
+      <c r="R89" s="126"/>
       <c r="S89" s="65"/>
       <c r="T89" s="26" t="s">
         <v>317</v>
@@ -5057,7 +5062,7 @@
       </c>
     </row>
     <row r="90" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="R90" s="73"/>
+      <c r="R90" s="126"/>
       <c r="S90" s="65"/>
       <c r="T90" s="26" t="s">
         <v>318</v>
@@ -5067,7 +5072,7 @@
       </c>
     </row>
     <row r="91" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="R91" s="73"/>
+      <c r="R91" s="126"/>
       <c r="S91" s="65"/>
       <c r="T91" s="26" t="s">
         <v>319</v>
@@ -5076,8 +5081,8 @@
         <v>328</v>
       </c>
     </row>
-    <row r="92" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R92" s="74"/>
+    <row r="92" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R92" s="127"/>
       <c r="S92" s="66"/>
       <c r="T92" s="18" t="s">
         <v>320</v>
@@ -5087,7 +5092,7 @@
       </c>
     </row>
     <row r="93" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="R93" s="72" t="s">
+      <c r="R93" s="125" t="s">
         <v>330</v>
       </c>
       <c r="S93" s="64" t="s">
@@ -5101,7 +5106,7 @@
       </c>
     </row>
     <row r="94" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="R94" s="73"/>
+      <c r="R94" s="126"/>
       <c r="S94" s="65" t="s">
         <v>411</v>
       </c>
@@ -5113,7 +5118,7 @@
       </c>
     </row>
     <row r="95" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="R95" s="73"/>
+      <c r="R95" s="126"/>
       <c r="S95" s="65" t="s">
         <v>412</v>
       </c>
@@ -5125,7 +5130,7 @@
       </c>
     </row>
     <row r="96" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="R96" s="73"/>
+      <c r="R96" s="126"/>
       <c r="S96" s="65" t="s">
         <v>413</v>
       </c>
@@ -5137,7 +5142,7 @@
       </c>
     </row>
     <row r="97" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R97" s="73"/>
+      <c r="R97" s="126"/>
       <c r="S97" s="65" t="s">
         <v>414</v>
       </c>
@@ -5149,7 +5154,7 @@
       </c>
     </row>
     <row r="98" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R98" s="73"/>
+      <c r="R98" s="126"/>
       <c r="S98" s="65" t="s">
         <v>415</v>
       </c>
@@ -5161,7 +5166,7 @@
       </c>
     </row>
     <row r="99" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R99" s="73"/>
+      <c r="R99" s="126"/>
       <c r="S99" s="65" t="s">
         <v>416</v>
       </c>
@@ -5173,7 +5178,7 @@
       </c>
     </row>
     <row r="100" spans="18:21" x14ac:dyDescent="0.25">
-      <c r="R100" s="73"/>
+      <c r="R100" s="126"/>
       <c r="S100" s="65" t="s">
         <v>417</v>
       </c>
@@ -5184,8 +5189,8 @@
         <v>347</v>
       </c>
     </row>
-    <row r="101" spans="18:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R101" s="74"/>
+    <row r="101" spans="18:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R101" s="127"/>
       <c r="S101" s="66" t="s">
         <v>418</v>
       </c>
@@ -5197,41 +5202,54 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="95">
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="J84:K84"/>
-    <mergeCell ref="J85:K85"/>
-    <mergeCell ref="J86:K86"/>
-    <mergeCell ref="J78:K78"/>
-    <mergeCell ref="J79:K79"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="J73:K73"/>
-    <mergeCell ref="J74:K74"/>
-    <mergeCell ref="J75:K75"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="J77:K77"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J71:K71"/>
-    <mergeCell ref="J72:K72"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="J57:K57"/>
+  <mergeCells count="97">
+    <mergeCell ref="R84:R92"/>
+    <mergeCell ref="R93:R101"/>
+    <mergeCell ref="R48:R56"/>
+    <mergeCell ref="R57:R65"/>
+    <mergeCell ref="R66:R74"/>
+    <mergeCell ref="R75:R83"/>
+    <mergeCell ref="R3:R11"/>
+    <mergeCell ref="R12:R20"/>
+    <mergeCell ref="R21:R29"/>
+    <mergeCell ref="R30:R38"/>
+    <mergeCell ref="R39:R47"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="B41:B48"/>
+    <mergeCell ref="C41:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="J49:K49"/>
     <mergeCell ref="J50:K50"/>
     <mergeCell ref="J51:K51"/>
@@ -5248,51 +5266,40 @@
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="B41:B48"/>
-    <mergeCell ref="C41:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="R3:R11"/>
-    <mergeCell ref="R12:R20"/>
-    <mergeCell ref="R21:R29"/>
-    <mergeCell ref="R30:R38"/>
-    <mergeCell ref="R39:R47"/>
-    <mergeCell ref="R84:R92"/>
-    <mergeCell ref="R93:R101"/>
-    <mergeCell ref="R48:R56"/>
-    <mergeCell ref="R57:R65"/>
-    <mergeCell ref="R66:R74"/>
-    <mergeCell ref="R75:R83"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="J72:K72"/>
+    <mergeCell ref="J73:K73"/>
+    <mergeCell ref="J74:K74"/>
+    <mergeCell ref="J75:K75"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="J77:K77"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="J85:K85"/>
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="J78:K78"/>
+    <mergeCell ref="J79:K79"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="J82:K82"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J27" r:id="rId1" display="http://acces.ens-lyon.fr" xr:uid="{BEC0A433-4355-432D-B5CD-3BE2EA5007B7}"/>

</xml_diff>